<commit_message>
sketched a mod matrix
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/mayafe_ntnu_no/Documents/Thesis/Project/code/ModMatrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BAF776A8-4C87-481C-9665-EE6641D5D1F3}"/>
+  <xr:revisionPtr revIDLastSave="57" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{12474056-32FF-40A7-A498-31E7B52529B4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>LFO</t>
   </si>
@@ -44,19 +44,19 @@
     <t>Expr.</t>
   </si>
   <si>
-    <t>Parm1</t>
-  </si>
-  <si>
-    <t>Parm2</t>
-  </si>
-  <si>
-    <t>Parm3</t>
-  </si>
-  <si>
     <t>Noisy</t>
   </si>
   <si>
-    <t>Wide</t>
+    <t>LFOFreq</t>
+  </si>
+  <si>
+    <t>Scale.Coeff</t>
+  </si>
+  <si>
+    <t>Freq</t>
+  </si>
+  <si>
+    <t>Cutoff</t>
   </si>
 </sst>
 </file>
@@ -118,6 +118,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -439,36 +443,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B57F66-A976-4D4A-AAE9-8652E91F323D}">
   <dimension ref="A1:S7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="18" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
@@ -481,10 +467,16 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="K2" s="1"/>
       <c r="P2" s="1"/>
@@ -493,11 +485,31 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>1</v>
+      <c r="B3">
+        <v>100</v>
+      </c>
+      <c r="C3">
+        <v>500</v>
+      </c>
+      <c r="D3">
+        <v>5</v>
       </c>
       <c r="K3" s="1"/>
       <c r="P3" s="1"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>

</xml_diff>

<commit_message>
created excel to python script
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/mayafe_ntnu_no/Documents/Thesis/Project/code/ModMatrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="58" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{69362CF9-3D4D-4C8B-B0BC-02886C8428A3}"/>
+  <xr:revisionPtr revIDLastSave="131" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D87BFB9C-10EF-42A0-8EB7-73023579E541}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="Comments" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,14 +37,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>LFO</t>
   </si>
   <si>
-    <t>Expr.</t>
-  </si>
-  <si>
     <t>Noisy</t>
   </si>
   <si>
@@ -57,6 +55,39 @@
   </si>
   <si>
     <t>Cutoff</t>
+  </si>
+  <si>
+    <t>Roomy</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>0-1</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>MixX</t>
+  </si>
+  <si>
+    <t>MixY</t>
+  </si>
+  <si>
+    <t>1 - morphX</t>
+  </si>
+  <si>
+    <t>"=morphX"</t>
+  </si>
+  <si>
+    <t>Expression</t>
+  </si>
+  <si>
+    <t>MorphX</t>
+  </si>
+  <si>
+    <t>MorphY</t>
   </si>
 </sst>
 </file>
@@ -441,106 +472,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B57F66-A976-4D4A-AAE9-8652E91F323D}">
-  <dimension ref="A1:S7"/>
+  <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="2" width="18" customWidth="1"/>
+    <col min="9" max="10" width="12.42578125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="1"/>
+      <c r="G1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
-      <c r="P1" s="1"/>
+      <c r="O1" s="1"/>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T1" s="1"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="L2" s="1"/>
+      <c r="Q2" s="1"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="1"/>
+      <c r="Q3" s="1"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>100</v>
+      </c>
+      <c r="E4">
+        <v>500</v>
+      </c>
+      <c r="F4">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>100</v>
-      </c>
-      <c r="C3">
-        <v>500</v>
-      </c>
-      <c r="D3">
-        <v>5</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4">
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>10</v>
       </c>
-      <c r="C4">
+      <c r="E5">
         <v>50</v>
       </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5">
+        <v>0</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="K5" s="1"/>
+      <c r="J5" s="1"/>
       <c r="L5" s="1"/>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-      <c r="P5" s="1"/>
+      <c r="O5" s="1"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="K6" s="1"/>
-      <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="T5" s="1"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="G6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="Q6" s="1"/>
+    </row>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="K7" s="1"/>
-      <c r="P7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="Q7" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5255341-57AC-4E26-8229-6395D70ACEA8}">
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
python script now writes the necessary  csound code based on the excel sheet. so the excel sheet can be used to edit the mapping
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/mayafe_ntnu_no/Documents/Thesis/Project/code/ModMatrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D87BFB9C-10EF-42A0-8EB7-73023579E541}"/>
+  <xr:revisionPtr revIDLastSave="133" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7E5F6AF-EB37-470E-BD18-9DC5C99E878D}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
   </bookViews>
@@ -475,7 +475,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
converter now writes to include file
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/mayafe_ntnu_no/Documents/Thesis/Project/code/ModMatrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C37591C0-0901-4C8B-B3A2-83A9BAD1B5DB}"/>
+  <xr:revisionPtr revIDLastSave="145" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94AA80E2-B771-4444-B338-5B30A4EBD44B}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
   <si>
     <t>LFO</t>
   </si>
@@ -88,12 +88,6 @@
   </si>
   <si>
     <t>MorphY</t>
-  </si>
-  <si>
-    <t>sfsdf</t>
-  </si>
-  <si>
-    <t>sdfsdf</t>
   </si>
 </sst>
 </file>
@@ -481,7 +475,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,18 +504,10 @@
       <c r="F1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
@@ -550,18 +536,6 @@
       <c r="F2">
         <v>0</v>
       </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-      <c r="H2">
-        <v>34</v>
-      </c>
-      <c r="I2">
-        <v>3</v>
-      </c>
-      <c r="J2">
-        <v>0</v>
-      </c>
       <c r="L2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
@@ -584,18 +558,6 @@
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-      <c r="H3">
-        <v>34</v>
-      </c>
-      <c r="I3">
-        <v>3</v>
-      </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
       <c r="L3" s="1"/>
       <c r="Q3" s="1"/>
     </row>
@@ -618,18 +580,6 @@
       <c r="F4">
         <v>5</v>
       </c>
-      <c r="G4">
-        <v>1</v>
-      </c>
-      <c r="H4">
-        <v>34</v>
-      </c>
-      <c r="I4">
-        <v>3</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
@@ -648,18 +598,6 @@
         <v>50</v>
       </c>
       <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>1</v>
-      </c>
-      <c r="H5">
-        <v>34</v>
-      </c>
-      <c r="I5">
-        <v>3</v>
-      </c>
-      <c r="J5">
         <v>0</v>
       </c>
       <c r="L5" s="1"/>

</xml_diff>

<commit_message>
added simple x control for two sound files
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/mayafe_ntnu_no/Documents/Thesis/Project/code/ModMatrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{94AA80E2-B771-4444-B338-5B30A4EBD44B}"/>
+  <xr:revisionPtr revIDLastSave="147" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9A0C4DD-20E7-4C9D-B66D-9BF7D792E3B7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
   </bookViews>
@@ -475,7 +475,7 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
fixed a bug (forgot to change parameter count in modmatrix.csd)
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/mayafe_ntnu_no/Documents/Thesis/Project/code/ModMatrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="147" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A9A0C4DD-20E7-4C9D-B66D-9BF7D792E3B7}"/>
+  <xr:revisionPtr revIDLastSave="208" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0393A21F-B49E-4B34-A5B7-6C4EDC4046F2}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
   <si>
     <t>LFO</t>
   </si>
@@ -88,13 +88,22 @@
   </si>
   <si>
     <t>MorphY</t>
+  </si>
+  <si>
+    <t>GrainRate</t>
+  </si>
+  <si>
+    <t>Preset1</t>
+  </si>
+  <si>
+    <t>Preset2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,16 +119,52 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -127,15 +172,85 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="4">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -475,151 +590,185 @@
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="18" customWidth="1"/>
-    <col min="9" max="10" width="12.42578125" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18" style="2" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="2"/>
+    <col min="4" max="4" width="13.85546875" style="2" customWidth="1"/>
+    <col min="5" max="8" width="9.140625" style="2"/>
+    <col min="9" max="10" width="12.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="9.140625" style="2"/>
+    <col min="12" max="12" width="14.28515625" style="2" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="D1" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D2" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-      <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="G2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="L2" s="4"/>
+      <c r="Q2" s="4"/>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="3">
         <v>1</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="1"/>
-      <c r="Q2" s="1"/>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="6">
+        <v>10</v>
+      </c>
+      <c r="E3" s="6">
+        <v>0</v>
+      </c>
+      <c r="F3" s="6">
+        <v>0</v>
+      </c>
+      <c r="G3" s="7">
+        <v>0</v>
+      </c>
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="L3" s="4"/>
+      <c r="Q3" s="4"/>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
+      <c r="B4" s="3">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
         <v>1</v>
       </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="1"/>
-      <c r="Q3" s="1"/>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="D4" s="6">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>0</v>
+      </c>
+      <c r="F4" s="6">
+        <v>0</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0</v>
+      </c>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4">
-        <v>0</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
+      <c r="B5" s="3">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="6">
         <v>100</v>
       </c>
-      <c r="E4">
+      <c r="E5" s="6">
         <v>500</v>
       </c>
-      <c r="F4">
+      <c r="F5" s="6">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
+      <c r="G5" s="7">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="4"/>
+      <c r="O5" s="4"/>
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4"/>
+      <c r="S5" s="4"/>
+      <c r="T5" s="4"/>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="3">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="6">
         <v>10</v>
       </c>
-      <c r="E5">
+      <c r="E6" s="6">
         <v>50</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1"/>
-      <c r="M5" s="1"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="Q5" s="1"/>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1"/>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="G6" s="1"/>
-      <c r="L6" s="1"/>
-      <c r="Q6" s="1"/>
+      <c r="F6" s="6">
+        <v>0</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="L6" s="4"/>
+      <c r="Q6" s="4"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="G7" s="1"/>
-      <c r="L7" s="1"/>
-      <c r="Q7" s="1"/>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="Q7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated convert.py so it adapts to size of excel file completely
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/mayafe_ntnu_no/Documents/Thesis/Project/code/ModMatrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="208" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0393A21F-B49E-4B34-A5B7-6C4EDC4046F2}"/>
+  <xr:revisionPtr revIDLastSave="219" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B6D86FD7-E50A-403E-B9F2-7D742B2BA6EA}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>LFO</t>
   </si>
@@ -90,13 +90,7 @@
     <t>MorphY</t>
   </si>
   <si>
-    <t>GrainRate</t>
-  </si>
-  <si>
     <t>Preset1</t>
-  </si>
-  <si>
-    <t>Preset2</t>
   </si>
 </sst>
 </file>
@@ -222,29 +216,26 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -264,10 +255,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -591,7 +578,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="K16" sqref="K16"/>
+      <selection pane="topRight" activeCell="L2" sqref="G2:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -609,26 +596,23 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="D1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="3"/>
+    </row>
+    <row r="2" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -643,19 +627,17 @@
       <c r="F2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="L2" s="4"/>
-      <c r="Q2" s="4"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="L2" s="3"/>
+      <c r="Q2" s="3"/>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="4">
         <v>1</v>
       </c>
       <c r="C3" s="5">
@@ -670,19 +652,17 @@
       <c r="F3" s="6">
         <v>0</v>
       </c>
-      <c r="G3" s="7">
-        <v>0</v>
-      </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="L3" s="4"/>
-      <c r="Q3" s="4"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="L3" s="3"/>
+      <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="4">
         <v>0</v>
       </c>
       <c r="C4" s="5">
@@ -697,17 +677,15 @@
       <c r="F4" s="6">
         <v>0</v>
       </c>
-      <c r="G4" s="7">
-        <v>0</v>
-      </c>
-      <c r="H4" s="8"/>
-      <c r="I4" s="8"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="4">
         <v>0</v>
       </c>
       <c r="C5" s="5">
@@ -722,25 +700,23 @@
       <c r="F5" s="6">
         <v>5</v>
       </c>
-      <c r="G5" s="7">
-        <v>0</v>
-      </c>
-      <c r="H5" s="8"/>
-      <c r="I5" s="8"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="4"/>
+      <c r="G5" s="7"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="3">
+      <c r="A6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="4">
         <v>0</v>
       </c>
       <c r="C6" s="5">
@@ -755,20 +731,18 @@
       <c r="F6" s="6">
         <v>0</v>
       </c>
-      <c r="G6" s="7">
-        <v>0</v>
-      </c>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="L6" s="4"/>
-      <c r="Q6" s="4"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="L6" s="3"/>
+      <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="Q7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="Q7" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fine tuning grain delay
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/mayafe_ntnu_no/Documents/Thesis/Project/code/ModMatrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="226" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E4814E0-96AD-4383-821A-3ACA4CF078D7}"/>
+  <xr:revisionPtr revIDLastSave="247" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36026B36-5D15-4759-B244-AF2A019B23D7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>LFO</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t>SendAmount</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>DistortAmount</t>
   </si>
 </sst>
 </file>
@@ -583,27 +589,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B57F66-A976-4D4A-AAE9-8652E91F323D}">
   <dimension ref="A1:T7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="63.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11" style="2" customWidth="1"/>
-    <col min="2" max="2" width="18" style="2" customWidth="1"/>
-    <col min="3" max="3" width="9.140625" style="2"/>
-    <col min="4" max="4" width="13.85546875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="9.140625" style="2"/>
-    <col min="6" max="6" width="14.7109375" style="2" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" style="2"/>
-    <col min="9" max="10" width="12.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="9.140625" style="2"/>
-    <col min="12" max="12" width="14.28515625" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="16384" width="12.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="2" t="s">
         <v>14</v>
       </c>
@@ -620,7 +615,7 @@
       <c r="S1" s="3"/>
       <c r="T1" s="3"/>
     </row>
-    <row r="2" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -639,13 +634,15 @@
       <c r="F2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="L2" s="3"/>
       <c r="Q2" s="3"/>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>12</v>
       </c>
@@ -670,7 +667,7 @@
       <c r="L3" s="3"/>
       <c r="Q3" s="3"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -693,7 +690,7 @@
       <c r="H4" s="7"/>
       <c r="I4" s="7"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
@@ -724,7 +721,7 @@
       <c r="S5" s="3"/>
       <c r="T5" s="3"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
@@ -749,7 +746,7 @@
       <c r="L6" s="3"/>
       <c r="Q6" s="3"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="G7" s="3"/>
@@ -758,20 +755,25 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5255341-57AC-4E26-8229-6395D70ACEA8}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
@@ -779,7 +781,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>9</v>
       </c>
@@ -787,7 +789,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -795,12 +797,20 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added generation of knobs in cabbage to prepare for modmatrix implementation
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/mayafe_ntnu_no/Documents/Thesis/Project/code/ModMatrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="247" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{36026B36-5D15-4759-B244-AF2A019B23D7}"/>
+  <xr:revisionPtr revIDLastSave="295" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBD9710C-CCB5-4745-BE3D-E324799C4CF4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>LFO</t>
   </si>
@@ -100,13 +100,31 @@
   </si>
   <si>
     <t>DistortAmount</t>
+  </si>
+  <si>
+    <t>Audiodescriptor1</t>
+  </si>
+  <si>
+    <t>Audiodescriptor2</t>
+  </si>
+  <si>
+    <t>Audiodescriptor3</t>
+  </si>
+  <si>
+    <t>LfoFreq</t>
+  </si>
+  <si>
+    <t>LfoAmp</t>
+  </si>
+  <si>
+    <t>Shape</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -139,6 +157,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -228,23 +252,23 @@
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -587,173 +611,315 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B57F66-A976-4D4A-AAE9-8652E91F323D}">
-  <dimension ref="A1:T7"/>
+  <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="63.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="12.140625" style="2"/>
+    <col min="1" max="16384" width="12.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
+      <c r="I1" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
     </row>
     <row r="2" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="L2" s="3"/>
-      <c r="Q2" s="3"/>
+      <c r="H2" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="7"/>
+      <c r="Q2" s="7"/>
     </row>
     <row r="3" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>1</v>
       </c>
-      <c r="C3" s="5">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
-        <v>0</v>
-      </c>
-      <c r="F3" s="6">
-        <v>0</v>
-      </c>
-      <c r="G3" s="7"/>
-      <c r="H3" s="7"/>
-      <c r="I3" s="7"/>
-      <c r="L3" s="3"/>
-      <c r="Q3" s="3"/>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7"/>
+      <c r="Q3" s="7"/>
     </row>
     <row r="4" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="5">
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6">
-        <v>0</v>
-      </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>20</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>20</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="4">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="6">
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
         <v>100</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E8" s="4">
         <v>500</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F8" s="4">
         <v>5</v>
       </c>
-      <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-    </row>
-    <row r="6" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6" s="4">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="L8" s="7"/>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+    </row>
+    <row r="9" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
         <v>10</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E9" s="4">
         <v>50</v>
       </c>
-      <c r="F6" s="6">
-        <v>0</v>
-      </c>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="L6" s="3"/>
-      <c r="Q6" s="3"/>
-    </row>
-    <row r="7" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="Q7" s="3"/>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0</v>
+      </c>
+      <c r="L9" s="7"/>
+      <c r="Q9" s="7"/>
+    </row>
+    <row r="10" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
+      <c r="B10" s="7"/>
+      <c r="G10" s="7"/>
+      <c r="L10" s="7"/>
+      <c r="Q10" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
input and output parameters are now reflected in UI
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/mayafe_ntnu_no/Documents/Thesis/Project/code/ModMatrix/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mayaf\OneDrive - NTNU\Thesis\Project\code\ModMatrix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="295" documentId="8_{0642ACC6-25DE-4137-9293-2416299506AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FBD9710C-CCB5-4745-BE3D-E324799C4CF4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397DFBAD-947D-40BD-A882-B430F9236050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>LFO</t>
   </si>
@@ -118,13 +118,16 @@
   </si>
   <si>
     <t>Shape</t>
+  </si>
+  <si>
+    <t>Smackidiboo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -288,10 +291,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -613,16 +612,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B57F66-A976-4D4A-AAE9-8652E91F323D}">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="63.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="63.75" customHeight="1"/>
   <cols>
-    <col min="1" max="16384" width="12.140625" style="6"/>
+    <col min="1" max="16384" width="12.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="63.75" customHeight="1">
       <c r="D1" s="6" t="s">
         <v>14</v>
       </c>
@@ -641,7 +640,7 @@
       <c r="S1" s="7"/>
       <c r="T1" s="7"/>
     </row>
-    <row r="2" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="63.75" customHeight="1">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -672,10 +671,13 @@
       <c r="J2" s="5" t="s">
         <v>25</v>
       </c>
+      <c r="K2" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="L2" s="7"/>
       <c r="Q2" s="7"/>
     </row>
-    <row r="3" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="63.75" customHeight="1">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
@@ -706,10 +708,13 @@
       <c r="J3" s="5">
         <v>0</v>
       </c>
+      <c r="K3" s="5">
+        <v>0</v>
+      </c>
       <c r="L3" s="7"/>
       <c r="Q3" s="7"/>
     </row>
-    <row r="4" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="63.75" customHeight="1">
       <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
@@ -740,8 +745,11 @@
       <c r="J4" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="63.75" customHeight="1">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
@@ -772,8 +780,11 @@
       <c r="J5" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="63.75" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
@@ -804,8 +815,11 @@
       <c r="J6" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="63.75" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
@@ -836,8 +850,11 @@
       <c r="J7" s="5">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="63.75" customHeight="1">
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
@@ -866,6 +883,9 @@
         <v>0</v>
       </c>
       <c r="J8" s="5">
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
         <v>0</v>
       </c>
       <c r="L8" s="7"/>
@@ -877,7 +897,7 @@
       <c r="S8" s="7"/>
       <c r="T8" s="7"/>
     </row>
-    <row r="9" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" ht="63.75" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
@@ -908,10 +928,13 @@
       <c r="J9" s="5">
         <v>0</v>
       </c>
+      <c r="K9" s="5">
+        <v>0</v>
+      </c>
       <c r="L9" s="7"/>
       <c r="Q9" s="7"/>
     </row>
-    <row r="10" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="63.75" customHeight="1">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="G10" s="7"/>
@@ -933,13 +956,13 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
@@ -947,7 +970,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="D2" t="s">
         <v>9</v>
       </c>
@@ -955,7 +978,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -963,7 +986,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -971,7 +994,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="E10" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
edits. Going to rework ui so it can be saved
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/mayafe_ntnu_no/Documents/Thesis/Project/code/ModMatrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{397DFBAD-947D-40BD-A882-B430F9236050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{34A20ADA-8ECE-4A5A-AD69-788936081314}"/>
+  <xr:revisionPtr revIDLastSave="112" documentId="13_ncr:1_{397DFBAD-947D-40BD-A882-B430F9236050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D8C21F2C-7944-4505-BF81-394C0C675CE8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
   <si>
     <t>LFO</t>
   </si>
@@ -118,19 +118,13 @@
   </si>
   <si>
     <t>Shape</t>
-  </si>
-  <si>
-    <t>Smackidiboo</t>
-  </si>
-  <si>
-    <t>Smudgirydoobidy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -294,6 +288,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -615,16 +613,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B57F66-A976-4D4A-AAE9-8652E91F323D}">
   <dimension ref="A1:T10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="63.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="63.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="12.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="63.75" customHeight="1">
+    <row r="1" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="6" t="s">
         <v>14</v>
       </c>
@@ -643,7 +641,7 @@
       <c r="S1" s="7"/>
       <c r="T1" s="7"/>
     </row>
-    <row r="2" spans="1:20" ht="63.75" customHeight="1">
+    <row r="2" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -674,290 +672,312 @@
       <c r="J2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="L2" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q2" s="7"/>
-    </row>
-    <row r="3" spans="1:20" ht="63.75" customHeight="1">
+      <c r="K2" s="2"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="4"/>
+      <c r="N2" s="4"/>
+      <c r="O2" s="4"/>
+      <c r="P2" s="2"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+      <c r="T2" s="4"/>
+    </row>
+    <row r="3" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C3" s="3">
-        <v>0</v>
+        <v>567</v>
       </c>
       <c r="D3" s="4">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E3" s="4">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="F3" s="4">
-        <v>0</v>
+        <v>434</v>
       </c>
       <c r="G3" s="5">
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="H3" s="5">
-        <v>0</v>
+        <v>235</v>
       </c>
       <c r="I3" s="5">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="J3" s="5">
-        <v>0</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0</v>
-      </c>
-      <c r="L3" s="5">
-        <v>32</v>
-      </c>
-      <c r="Q3" s="7"/>
-    </row>
-    <row r="4" spans="1:20" ht="63.75" customHeight="1">
+        <v>324234</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+    </row>
+    <row r="4" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C4" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D4" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E4" s="4">
-        <v>0</v>
+        <v>46</v>
       </c>
       <c r="F4" s="4">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="G4" s="5">
-        <v>0</v>
+        <v>77</v>
       </c>
       <c r="H4" s="5">
-        <v>0</v>
+        <v>453</v>
       </c>
       <c r="I4" s="5">
-        <v>0</v>
+        <v>543</v>
       </c>
       <c r="J4" s="5">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0</v>
-      </c>
-      <c r="L4" s="5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="63.75" customHeight="1">
+        <v>23546</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+    </row>
+    <row r="5" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>21</v>
       </c>
       <c r="B5" s="2">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="C5" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="D5" s="4">
-        <v>0</v>
+        <v>5656</v>
       </c>
       <c r="E5" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F5" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G5" s="5">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="H5" s="5">
-        <v>0</v>
+        <v>46546</v>
       </c>
       <c r="I5" s="5">
-        <v>20</v>
+        <v>534</v>
       </c>
       <c r="J5" s="5">
-        <v>0</v>
-      </c>
-      <c r="K5" s="5">
-        <v>0</v>
-      </c>
-      <c r="L5" s="5">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="63.75" customHeight="1">
+        <v>67776767</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+    </row>
+    <row r="6" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B6" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="C6" s="2">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="D6" s="4">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="E6" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F6" s="4">
-        <v>0</v>
+        <v>43</v>
       </c>
       <c r="G6" s="5">
-        <v>0</v>
+        <v>99</v>
       </c>
       <c r="H6" s="5">
-        <v>0</v>
+        <v>767</v>
       </c>
       <c r="I6" s="5">
-        <v>20</v>
+        <v>534</v>
       </c>
       <c r="J6" s="5">
-        <v>0</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0</v>
-      </c>
-      <c r="L6" s="5">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="63.75" customHeight="1">
+        <v>6778987</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+    </row>
+    <row r="7" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
         <v>23</v>
       </c>
       <c r="B7" s="2">
-        <v>0</v>
+        <v>323</v>
       </c>
       <c r="C7" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D7" s="4">
-        <v>0</v>
+        <v>534</v>
       </c>
       <c r="E7" s="4">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="4">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="G7" s="5">
-        <v>0</v>
+        <v>88</v>
       </c>
       <c r="H7" s="5">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="I7" s="5">
-        <v>0</v>
+        <v>534</v>
       </c>
       <c r="J7" s="5">
-        <v>0</v>
-      </c>
-      <c r="K7" s="5">
-        <v>0</v>
-      </c>
-      <c r="L7" s="5">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="63.75" customHeight="1">
+        <v>789</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+    </row>
+    <row r="8" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="2">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D8" s="4">
-        <v>100</v>
+        <v>24</v>
       </c>
       <c r="E8" s="4">
-        <v>500</v>
+        <v>3</v>
       </c>
       <c r="F8" s="4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G8" s="5">
-        <v>0</v>
+        <v>55</v>
       </c>
       <c r="H8" s="5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="I8" s="5">
-        <v>0</v>
+        <v>534</v>
       </c>
       <c r="J8" s="5">
-        <v>0</v>
-      </c>
-      <c r="K8" s="5">
-        <v>0</v>
-      </c>
-      <c r="L8" s="5">
-        <v>0</v>
-      </c>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-    </row>
-    <row r="9" spans="1:20" ht="63.75" customHeight="1">
+        <v>879</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+      <c r="M8" s="5"/>
+      <c r="N8" s="5"/>
+      <c r="O8" s="5"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+    </row>
+    <row r="9" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B9" s="2">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C9" s="3">
         <v>0</v>
       </c>
       <c r="D9" s="4">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E9" s="4">
-        <v>50</v>
+        <v>5</v>
       </c>
       <c r="F9" s="4">
         <v>0</v>
       </c>
       <c r="G9" s="5">
-        <v>0</v>
+        <v>345</v>
       </c>
       <c r="H9" s="5">
-        <v>0</v>
+        <v>4534</v>
       </c>
       <c r="I9" s="5">
-        <v>0</v>
+        <v>534</v>
       </c>
       <c r="J9" s="5">
-        <v>0</v>
-      </c>
-      <c r="K9" s="5">
-        <v>0</v>
-      </c>
-      <c r="L9" s="5">
-        <v>4</v>
-      </c>
-      <c r="Q9" s="7"/>
-    </row>
-    <row r="10" spans="1:20" ht="63.75" customHeight="1">
+        <v>78</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5"/>
+      <c r="M9" s="5"/>
+      <c r="N9" s="5"/>
+      <c r="O9" s="5"/>
+      <c r="P9" s="5"/>
+      <c r="Q9" s="5"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+    </row>
+    <row r="10" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="G10" s="7"/>
@@ -979,13 +999,13 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
@@ -993,7 +1013,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>9</v>
       </c>
@@ -1001,7 +1021,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1009,7 +1029,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1017,7 +1037,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
gotta figure out how parameters can be mapped in reaper
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -294,6 +294,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>

<commit_message>
added connection to audio analyser by hardcoding audiodescriptors
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/mayafe_ntnu_no/Documents/Thesis/Project/code/ModMatrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="13_ncr:1_{397DFBAD-947D-40BD-A882-B430F9236050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8327FAB-70BF-4123-B0BF-1FD4C64D615B}"/>
+  <xr:revisionPtr revIDLastSave="144" documentId="13_ncr:1_{397DFBAD-947D-40BD-A882-B430F9236050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07040EE6-14DD-4D45-8CEF-69B3A9B5AA2A}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t>"=morphX"</t>
   </si>
   <si>
-    <t>Expression</t>
-  </si>
-  <si>
     <t>MorphX</t>
   </si>
   <si>
@@ -120,17 +117,20 @@
     <t>Shape</t>
   </si>
   <si>
-    <t>Smackidiboo</t>
-  </si>
-  <si>
-    <t>Smudgirydoobidy</t>
+    <t>Audiodescriptor4</t>
+  </si>
+  <si>
+    <t>Audiodescriptor5</t>
+  </si>
+  <si>
+    <t>Audiodescriptor6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -617,23 +617,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B57F66-A976-4D4A-AAE9-8652E91F323D}">
-  <dimension ref="A1:T10"/>
+  <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="59" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:L9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q3" sqref="P3:Q3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="63.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="63.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="12.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="63.75" customHeight="1">
+    <row r="1" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>14</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>15</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>0</v>
@@ -647,7 +647,7 @@
       <c r="S1" s="7"/>
       <c r="T1" s="7"/>
     </row>
-    <row r="2" spans="1:20" ht="63.75" customHeight="1">
+    <row r="2" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -658,315 +658,325 @@
         <v>8</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="F2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>18</v>
-      </c>
       <c r="G2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" s="7"/>
+    </row>
+    <row r="3" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0</v>
+      </c>
+      <c r="C3" s="3">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4">
+        <v>0</v>
+      </c>
+      <c r="E3" s="4">
+        <v>0</v>
+      </c>
+      <c r="F3" s="4">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3" s="7"/>
+    </row>
+    <row r="4" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0</v>
+      </c>
+      <c r="D4" s="4">
+        <v>0</v>
+      </c>
+      <c r="E4" s="4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0</v>
+      </c>
+      <c r="H4" s="5">
+        <v>0</v>
+      </c>
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="K2" s="5" t="s">
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="B9" s="2">
+        <v>0</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
+      <c r="I9" s="5">
+        <v>0</v>
+      </c>
+      <c r="J9" s="5">
+        <v>0</v>
+      </c>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+      <c r="M9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+    </row>
+    <row r="10" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="7"/>
-    </row>
-    <row r="3" spans="1:20" ht="63.75" customHeight="1">
-      <c r="A3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="2">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3">
-        <v>0</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0</v>
-      </c>
-      <c r="G3" s="5">
-        <v>0</v>
-      </c>
-      <c r="H3" s="5">
-        <v>0</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0</v>
-      </c>
-      <c r="L3" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="7"/>
-    </row>
-    <row r="4" spans="1:20" ht="63.75" customHeight="1">
-      <c r="A4" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="2">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>0</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="G4" s="5">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>0</v>
-      </c>
-      <c r="I4" s="5">
-        <v>0</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0</v>
-      </c>
-      <c r="L4" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" ht="63.75" customHeight="1">
-      <c r="A5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="5">
-        <v>0</v>
-      </c>
-      <c r="K5" s="5">
-        <v>0</v>
-      </c>
-      <c r="L5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" ht="63.75" customHeight="1">
-      <c r="A6" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0</v>
-      </c>
-      <c r="K6" s="5">
-        <v>0</v>
-      </c>
-      <c r="L6" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" ht="63.75" customHeight="1">
-      <c r="A7" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5">
-        <v>0</v>
-      </c>
-      <c r="K7" s="5">
-        <v>0</v>
-      </c>
-      <c r="L7" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="63.75" customHeight="1">
-      <c r="A8" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0</v>
-      </c>
-      <c r="K8" s="5">
-        <v>0</v>
-      </c>
-      <c r="L8" s="5">
-        <v>0</v>
-      </c>
-      <c r="M8" s="7"/>
-      <c r="N8" s="7"/>
-      <c r="O8" s="7"/>
-      <c r="Q8" s="7"/>
-      <c r="R8" s="7"/>
-      <c r="S8" s="7"/>
-      <c r="T8" s="7"/>
-    </row>
-    <row r="9" spans="1:20" ht="63.75" customHeight="1">
-      <c r="A9" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="2">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3">
-        <v>0</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>0</v>
-      </c>
-      <c r="G9" s="5">
-        <v>0</v>
-      </c>
-      <c r="H9" s="5">
-        <v>0</v>
-      </c>
-      <c r="I9" s="5">
-        <v>0</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0</v>
-      </c>
-      <c r="K9" s="5">
-        <v>0</v>
-      </c>
-      <c r="L9" s="5">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="7"/>
-    </row>
-    <row r="10" spans="1:20" ht="63.75" customHeight="1">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="G10" s="7"/>
-      <c r="L10" s="7"/>
-      <c r="Q10" s="7"/>
+      <c r="B10" s="2">
+        <v>0</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <v>0</v>
+      </c>
+      <c r="J10" s="5">
+        <v>0</v>
+      </c>
+      <c r="O10" s="7"/>
+    </row>
+    <row r="11" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="2">
+        <v>0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>0</v>
+      </c>
+      <c r="D11" s="4">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="O11" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -983,13 +993,13 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="16.5703125" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
@@ -997,7 +1007,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
         <v>9</v>
       </c>
@@ -1005,7 +1015,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1013,7 +1023,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1021,9 +1031,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F10">
         <v>1</v>

</xml_diff>

<commit_message>
added metro to osc reading
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/mayafe_ntnu_no/Documents/Thesis/Project/code/ModMatrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="13_ncr:1_{397DFBAD-947D-40BD-A882-B430F9236050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{07040EE6-14DD-4D45-8CEF-69B3A9B5AA2A}"/>
+  <xr:revisionPtr revIDLastSave="164" documentId="13_ncr:1_{397DFBAD-947D-40BD-A882-B430F9236050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EF4F9E6-3D52-4884-BC1C-CEF53B30424E}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>LFO</t>
   </si>
@@ -60,12 +60,6 @@
     <t>y</t>
   </si>
   <si>
-    <t>MixX</t>
-  </si>
-  <si>
-    <t>MixY</t>
-  </si>
-  <si>
     <t>1 - morphX</t>
   </si>
   <si>
@@ -84,21 +78,9 @@
     <t>Noise</t>
   </si>
   <si>
-    <t>Delay</t>
-  </si>
-  <si>
-    <t>LPF</t>
-  </si>
-  <si>
-    <t>SendAmount</t>
-  </si>
-  <si>
     <t>0,0</t>
   </si>
   <si>
-    <t>DistortAmount</t>
-  </si>
-  <si>
     <t>Audiodescriptor1</t>
   </si>
   <si>
@@ -108,15 +90,6 @@
     <t>Audiodescriptor3</t>
   </si>
   <si>
-    <t>LfoFreq</t>
-  </si>
-  <si>
-    <t>LfoAmp</t>
-  </si>
-  <si>
-    <t>Shape</t>
-  </si>
-  <si>
     <t>Audiodescriptor4</t>
   </si>
   <si>
@@ -124,6 +97,30 @@
   </si>
   <si>
     <t>Audiodescriptor6</t>
+  </si>
+  <si>
+    <t>/track/1/fx/1/fxparam/1/value</t>
+  </si>
+  <si>
+    <t>/track/1/fx/1/fxparam/2/value</t>
+  </si>
+  <si>
+    <t>/track/1/fx/1/fxparam/3/value</t>
+  </si>
+  <si>
+    <t>/track/1/fx/1/fxparam/4/value</t>
+  </si>
+  <si>
+    <t>/track/1/fx/2/fxparam/1/value</t>
+  </si>
+  <si>
+    <t>/track/1/fx/2/fxparam/2/value</t>
+  </si>
+  <si>
+    <t>/track/1/fx/3/fxparam/3/value</t>
+  </si>
+  <si>
+    <t>/track/1/fx/4/fxparam/4/value</t>
   </si>
 </sst>
 </file>
@@ -620,20 +617,29 @@
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Q3" sqref="P3:Q3"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="63.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="12.140625" style="6"/>
+    <col min="1" max="1" width="12.140625" style="6"/>
+    <col min="2" max="2" width="43.28515625" style="6" customWidth="1"/>
+    <col min="3" max="4" width="12.140625" style="6"/>
+    <col min="5" max="5" width="38.7109375" style="6" customWidth="1"/>
+    <col min="6" max="6" width="15.28515625" style="6" customWidth="1"/>
+    <col min="7" max="7" width="31.5703125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="22.85546875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="23.5703125" style="6" customWidth="1"/>
+    <col min="10" max="10" width="36.5703125" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="12.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D1" s="6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>0</v>
@@ -652,37 +658,35 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>8</v>
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="H2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>24</v>
-      </c>
+      <c r="H2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="5"/>
       <c r="O2" s="7"/>
     </row>
     <row r="3" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -708,14 +712,12 @@
       <c r="I3" s="5">
         <v>0</v>
       </c>
-      <c r="J3" s="5">
-        <v>0</v>
-      </c>
+      <c r="J3" s="5"/>
       <c r="O3" s="7"/>
     </row>
     <row r="4" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -741,13 +743,11 @@
       <c r="I4" s="5">
         <v>0</v>
       </c>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
+      <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -773,13 +773,11 @@
       <c r="I5" s="5">
         <v>0</v>
       </c>
-      <c r="J5" s="5">
-        <v>0</v>
-      </c>
+      <c r="J5" s="5"/>
     </row>
     <row r="6" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -805,13 +803,11 @@
       <c r="I6" s="5">
         <v>0</v>
       </c>
-      <c r="J6" s="5">
-        <v>0</v>
-      </c>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -837,13 +833,11 @@
       <c r="I7" s="5">
         <v>0</v>
       </c>
-      <c r="J7" s="5">
-        <v>0</v>
-      </c>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
@@ -869,13 +863,11 @@
       <c r="I8" s="5">
         <v>0</v>
       </c>
-      <c r="J8" s="5">
-        <v>0</v>
-      </c>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
@@ -901,9 +893,7 @@
       <c r="I9" s="5">
         <v>0</v>
       </c>
-      <c r="J9" s="5">
-        <v>0</v>
-      </c>
+      <c r="J9" s="5"/>
       <c r="K9" s="7"/>
       <c r="L9" s="7"/>
       <c r="M9" s="7"/>
@@ -914,7 +904,7 @@
     </row>
     <row r="10" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -940,9 +930,7 @@
       <c r="I10" s="5">
         <v>0</v>
       </c>
-      <c r="J10" s="5">
-        <v>0</v>
-      </c>
+      <c r="J10" s="5"/>
       <c r="O10" s="7"/>
     </row>
     <row r="11" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -973,9 +961,7 @@
       <c r="I11" s="5">
         <v>0</v>
       </c>
-      <c r="J11" s="5">
-        <v>0</v>
-      </c>
+      <c r="J11" s="5"/>
       <c r="O11" s="7"/>
     </row>
   </sheetData>
@@ -1009,10 +995,10 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1033,7 +1019,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E10" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="F10">
         <v>1</v>

</xml_diff>

<commit_message>
added mouse control of modmatrix for testing
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/mayafe_ntnu_no/Documents/Thesis/Project/code/ModMatrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="164" documentId="13_ncr:1_{397DFBAD-947D-40BD-A882-B430F9236050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EF4F9E6-3D52-4884-BC1C-CEF53B30424E}"/>
+  <xr:revisionPtr revIDLastSave="205" documentId="13_ncr:1_{397DFBAD-947D-40BD-A882-B430F9236050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC87E624-8B8B-4A4E-8CD2-CAB2EA21FE86}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -66,12 +66,6 @@
     <t>"=morphX"</t>
   </si>
   <si>
-    <t>MorphX</t>
-  </si>
-  <si>
-    <t>MorphY</t>
-  </si>
-  <si>
     <t>Reverb</t>
   </si>
   <si>
@@ -99,28 +93,34 @@
     <t>Audiodescriptor6</t>
   </si>
   <si>
-    <t>/track/1/fx/1/fxparam/1/value</t>
-  </si>
-  <si>
-    <t>/track/1/fx/1/fxparam/2/value</t>
-  </si>
-  <si>
-    <t>/track/1/fx/1/fxparam/3/value</t>
-  </si>
-  <si>
-    <t>/track/1/fx/1/fxparam/4/value</t>
-  </si>
-  <si>
-    <t>/track/1/fx/2/fxparam/1/value</t>
-  </si>
-  <si>
-    <t>/track/1/fx/2/fxparam/2/value</t>
-  </si>
-  <si>
-    <t>/track/1/fx/3/fxparam/3/value</t>
-  </si>
-  <si>
-    <t>/track/1/fx/4/fxparam/4/value</t>
+    <t>Mousex</t>
+  </si>
+  <si>
+    <t>Mousey</t>
+  </si>
+  <si>
+    <t>GrainRate</t>
+  </si>
+  <si>
+    <t>Duration</t>
+  </si>
+  <si>
+    <t>Freq</t>
+  </si>
+  <si>
+    <t>FmPitch</t>
+  </si>
+  <si>
+    <t>FmIndex</t>
+  </si>
+  <si>
+    <t>Env</t>
+  </si>
+  <si>
+    <t>RndMask</t>
+  </si>
+  <si>
+    <t>Distr</t>
   </si>
 </sst>
 </file>
@@ -617,29 +617,29 @@
   <dimension ref="A1:T11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:J1048576"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.140625" defaultRowHeight="63.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="63.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="6"/>
-    <col min="2" max="2" width="43.28515625" style="6" customWidth="1"/>
-    <col min="3" max="4" width="12.140625" style="6"/>
-    <col min="5" max="5" width="38.7109375" style="6" customWidth="1"/>
-    <col min="6" max="6" width="15.28515625" style="6" customWidth="1"/>
-    <col min="7" max="7" width="31.5703125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="22.85546875" style="6" customWidth="1"/>
-    <col min="9" max="9" width="23.5703125" style="6" customWidth="1"/>
-    <col min="10" max="10" width="36.5703125" style="6" customWidth="1"/>
-    <col min="11" max="16384" width="12.140625" style="6"/>
+    <col min="1" max="1" width="12.109375" style="6"/>
+    <col min="2" max="2" width="43.33203125" style="6" customWidth="1"/>
+    <col min="3" max="4" width="12.109375" style="6"/>
+    <col min="5" max="5" width="38.6640625" style="6" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" style="6" customWidth="1"/>
+    <col min="7" max="7" width="31.5546875" style="6" customWidth="1"/>
+    <col min="8" max="8" width="22.88671875" style="6" customWidth="1"/>
+    <col min="9" max="9" width="23.5546875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="36.5546875" style="6" customWidth="1"/>
+    <col min="11" max="16384" width="12.109375" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D1" s="6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="I1" s="7" t="s">
         <v>0</v>
@@ -653,7 +653,7 @@
       <c r="S1" s="7"/>
       <c r="T1" s="7"/>
     </row>
-    <row r="2" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
@@ -676,17 +676,17 @@
         <v>25</v>
       </c>
       <c r="H2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>26</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>27</v>
       </c>
       <c r="J2" s="5"/>
       <c r="O2" s="7"/>
     </row>
-    <row r="3" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -715,9 +715,9 @@
       <c r="J3" s="5"/>
       <c r="O3" s="7"/>
     </row>
-    <row r="4" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -745,129 +745,129 @@
       </c>
       <c r="J4" s="5"/>
     </row>
-    <row r="5" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0</v>
+      </c>
+      <c r="E5" s="4">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="5">
+        <v>0</v>
+      </c>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0</v>
+      </c>
+      <c r="D6" s="4">
+        <v>0</v>
+      </c>
+      <c r="E6" s="4">
+        <v>0</v>
+      </c>
+      <c r="F6" s="4">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0</v>
+      </c>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="2">
-        <v>0</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-      <c r="H5" s="5">
-        <v>0</v>
-      </c>
-      <c r="I5" s="5">
-        <v>0</v>
-      </c>
-      <c r="J5" s="5"/>
-    </row>
-    <row r="6" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="B7" s="2">
+        <v>0</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4">
+        <v>0</v>
+      </c>
+      <c r="F7" s="4">
+        <v>0</v>
+      </c>
+      <c r="G7" s="5">
+        <v>0</v>
+      </c>
+      <c r="H7" s="5">
+        <v>0</v>
+      </c>
+      <c r="I7" s="5">
+        <v>0</v>
+      </c>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B6" s="2">
-        <v>0</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
-      <c r="H6" s="5">
-        <v>0</v>
-      </c>
-      <c r="I6" s="5">
-        <v>0</v>
-      </c>
-      <c r="J6" s="5"/>
-    </row>
-    <row r="7" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="B8" s="2">
+        <v>0</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0</v>
+      </c>
+      <c r="D8" s="4">
+        <v>0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <v>0</v>
+      </c>
+      <c r="I8" s="5">
+        <v>0</v>
+      </c>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
         <v>16</v>
-      </c>
-      <c r="B7" s="2">
-        <v>0</v>
-      </c>
-      <c r="C7" s="2">
-        <v>0</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0</v>
-      </c>
-      <c r="G7" s="5">
-        <v>0</v>
-      </c>
-      <c r="H7" s="5">
-        <v>0</v>
-      </c>
-      <c r="I7" s="5">
-        <v>0</v>
-      </c>
-      <c r="J7" s="5"/>
-    </row>
-    <row r="8" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="2">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0</v>
-      </c>
-      <c r="F8" s="4">
-        <v>0</v>
-      </c>
-      <c r="G8" s="5">
-        <v>0</v>
-      </c>
-      <c r="H8" s="5">
-        <v>0</v>
-      </c>
-      <c r="I8" s="5">
-        <v>0</v>
-      </c>
-      <c r="J8" s="5"/>
-    </row>
-    <row r="9" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>18</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
@@ -902,9 +902,9 @@
       <c r="Q9" s="7"/>
       <c r="R9" s="7"/>
     </row>
-    <row r="10" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -933,7 +933,7 @@
       <c r="J10" s="5"/>
       <c r="O10" s="7"/>
     </row>
-    <row r="11" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7" t="s">
         <v>0</v>
       </c>
@@ -979,13 +979,13 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="16.5703125" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" customWidth="1"/>
+    <col min="5" max="5" width="22.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
@@ -993,7 +993,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
         <v>7</v>
       </c>
@@ -1001,7 +1001,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1009,7 +1009,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>6</v>
       </c>
@@ -1017,9 +1017,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="E10" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="F10">
         <v>1</v>

</xml_diff>

<commit_message>
fixed bug with audio descriptors. Variables named wrong after using convert.py again.
</commit_message>
<xml_diff>
--- a/ModMatrix/ModMatrixTable.xlsx
+++ b/ModMatrix/ModMatrixTable.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studntnu-my.sharepoint.com/personal/mayafe_ntnu_no/Documents/Thesis/Project/code/ModMatrix/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="205" documentId="13_ncr:1_{397DFBAD-947D-40BD-A882-B430F9236050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC87E624-8B8B-4A4E-8CD2-CAB2EA21FE86}"/>
+  <xr:revisionPtr revIDLastSave="218" documentId="13_ncr:1_{397DFBAD-947D-40BD-A882-B430F9236050}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C1B7BBC-594E-42D7-B7C8-8B7A89029E12}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{572823EF-07A5-4688-AF7A-282A01173643}"/>
   </bookViews>
@@ -75,24 +75,6 @@
     <t>0,0</t>
   </si>
   <si>
-    <t>Audiodescriptor1</t>
-  </si>
-  <si>
-    <t>Audiodescriptor2</t>
-  </si>
-  <si>
-    <t>Audiodescriptor3</t>
-  </si>
-  <si>
-    <t>Audiodescriptor4</t>
-  </si>
-  <si>
-    <t>Audiodescriptor5</t>
-  </si>
-  <si>
-    <t>Audiodescriptor6</t>
-  </si>
-  <si>
     <t>Mousex</t>
   </si>
   <si>
@@ -121,6 +103,24 @@
   </si>
   <si>
     <t>Distr</t>
+  </si>
+  <si>
+    <t>Rms</t>
+  </si>
+  <si>
+    <t>Pitch</t>
+  </si>
+  <si>
+    <t>Centroid</t>
+  </si>
+  <si>
+    <t>Flatness</t>
+  </si>
+  <si>
+    <t>TransDens</t>
+  </si>
+  <si>
+    <t>Spread</t>
   </si>
 </sst>
 </file>
@@ -291,10 +291,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -616,8 +612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88B57F66-A976-4D4A-AAE9-8652E91F323D}">
   <dimension ref="A1:T11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="63.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -658,35 +654,35 @@
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>20</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="J2" s="5"/>
       <c r="O2" s="7"/>
     </row>
     <row r="3" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2">
         <v>0</v>
@@ -717,7 +713,7 @@
     </row>
     <row r="4" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="7" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B4" s="2">
         <v>0</v>
@@ -747,7 +743,7 @@
     </row>
     <row r="5" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="7" t="s">
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -777,7 +773,7 @@
     </row>
     <row r="6" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="7" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -807,7 +803,7 @@
     </row>
     <row r="7" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="7" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2">
         <v>0</v>
@@ -837,7 +833,7 @@
     </row>
     <row r="8" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B8" s="2">
         <v>0</v>
@@ -867,7 +863,7 @@
     </row>
     <row r="9" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="7" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
@@ -904,7 +900,7 @@
     </row>
     <row r="10" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>

</xml_diff>